<commit_message>
add number of comment
</commit_message>
<xml_diff>
--- a/document/商品信息.xlsx
+++ b/document/商品信息.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{FF46B0FF-08DF-4D5F-9603-BAC9ED608507}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{5AF6EB52-01BB-4AE0-AC60-A0F8CD69C15C}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="135">
   <si>
     <t>价格</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -554,6 +554,10 @@
   </si>
   <si>
     <t>特别喜欢，很好，没想到像素也超级好</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>评论数</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -923,8 +927,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G27" sqref="G26:G27"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -964,7 +968,9 @@
       <c r="H1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="I1" s="1"/>
+      <c r="I1" s="1" t="s">
+        <v>134</v>
+      </c>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
     </row>
@@ -993,6 +999,9 @@
       <c r="H2" t="s">
         <v>13</v>
       </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:11" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -1019,6 +1028,9 @@
       <c r="H3" t="s">
         <v>13</v>
       </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:11" ht="81" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -1045,6 +1057,9 @@
       <c r="H4" t="s">
         <v>14</v>
       </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="1:11" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -1071,6 +1086,9 @@
       <c r="H5" t="s">
         <v>16</v>
       </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="1:11" ht="57" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -1097,6 +1115,9 @@
       <c r="H6" t="s">
         <v>17</v>
       </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:11" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -1123,6 +1144,9 @@
       <c r="H7" t="s">
         <v>18</v>
       </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
     </row>
     <row r="9" spans="1:11" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
@@ -1149,6 +1173,9 @@
       <c r="H9" t="s">
         <v>13</v>
       </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:11" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
@@ -1175,6 +1202,9 @@
       <c r="H10" t="s">
         <v>13</v>
       </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
     </row>
     <row r="11" spans="1:11" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
@@ -1201,6 +1231,9 @@
       <c r="H11" t="s">
         <v>14</v>
       </c>
+      <c r="I11">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="1:11" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
@@ -1227,6 +1260,9 @@
       <c r="H12" t="s">
         <v>16</v>
       </c>
+      <c r="I12">
+        <v>1</v>
+      </c>
     </row>
     <row r="13" spans="1:11" ht="57" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
@@ -1253,6 +1289,9 @@
       <c r="H13" t="s">
         <v>17</v>
       </c>
+      <c r="I13">
+        <v>1</v>
+      </c>
     </row>
     <row r="14" spans="1:11" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
@@ -1278,6 +1317,9 @@
       </c>
       <c r="H14" t="s">
         <v>18</v>
+      </c>
+      <c r="I14">
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
@@ -1310,8 +1352,11 @@
       <c r="H16" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" ht="57" x14ac:dyDescent="0.2">
+      <c r="I16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="57" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>85</v>
       </c>
@@ -1336,8 +1381,11 @@
       <c r="H17" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" ht="57" x14ac:dyDescent="0.2">
+      <c r="I17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="57" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>86</v>
       </c>
@@ -1362,8 +1410,11 @@
       <c r="H18" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" ht="71.25" x14ac:dyDescent="0.2">
+      <c r="I18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>87</v>
       </c>
@@ -1388,8 +1439,11 @@
       <c r="H19" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" ht="71.25" x14ac:dyDescent="0.2">
+      <c r="I19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>88</v>
       </c>
@@ -1414,8 +1468,11 @@
       <c r="H20" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="I20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>97</v>
       </c>
@@ -1440,8 +1497,11 @@
       <c r="H22" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="I22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>98</v>
       </c>
@@ -1466,8 +1526,11 @@
       <c r="H23" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" ht="99.75" x14ac:dyDescent="0.2">
+      <c r="I23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="99.75" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>103</v>
       </c>
@@ -1492,8 +1555,11 @@
       <c r="H25" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" ht="71.25" x14ac:dyDescent="0.2">
+      <c r="I25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>104</v>
       </c>
@@ -1518,8 +1584,11 @@
       <c r="H26" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" ht="99.75" x14ac:dyDescent="0.2">
+      <c r="I26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="99.75" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>105</v>
       </c>
@@ -1544,11 +1613,14 @@
       <c r="H27" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C28" s="3"/>
     </row>
-    <row r="29" spans="1:8" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>119</v>
       </c>
@@ -1573,8 +1645,11 @@
       <c r="H29" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="I29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>120</v>
       </c>
@@ -1599,8 +1674,11 @@
       <c r="H30" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="I30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>118</v>
       </c>
@@ -1624,6 +1702,9 @@
       </c>
       <c r="H31" t="s">
         <v>18</v>
+      </c>
+      <c r="I31">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>